<commit_message>
unit & int tests done
</commit_message>
<xml_diff>
--- a/data/input/test.xlsx
+++ b/data/input/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPAC-O-10\Documents\Opgaver\Uge4\PDFDownloader\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPAC-O-10\Documents\Opgaver\Uge5\PDFDownloaderTest\PDFDownloaderTest\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED3CCC2-E9FD-47DD-88E7-92DD5B267996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560834A5-0D7A-452E-95E6-1694F999470B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="27000" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="19" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="138">
   <si>
     <t>BRnum</t>
   </si>
@@ -453,273 +453,6 @@
   </si>
   <si>
     <t>http://database.globalreporting.org/reports/5a1f9f2b-fe6f-ea11-a811-000d3ab11761</t>
-  </si>
-  <si>
-    <t>BR50050</t>
-  </si>
-  <si>
-    <t>Aargauische Kantonalbank</t>
-  </si>
-  <si>
-    <t>Financial Services</t>
-  </si>
-  <si>
-    <t>1-6-2018</t>
-  </si>
-  <si>
-    <t>AKB Nachhaltigkeitsbericht 2016</t>
-  </si>
-  <si>
-    <t>Not Used</t>
-  </si>
-  <si>
-    <t>https://www.akb.ch/documents/30573/92310/nachhaltigkeitsbericht-2016.pdf</t>
-  </si>
-  <si>
-    <t>https://www.akb.ch/die-akb/kommunikation-medien/geschaeftsberichte</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/c3c6ed85-2a63-e811-8136-e0071b6641b1</t>
-  </si>
-  <si>
-    <t>BR50051</t>
-  </si>
-  <si>
-    <t>AB Klaipėdos Nafta</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>15-1-2018</t>
-  </si>
-  <si>
-    <t>2016 Social Responsibility Progress Report</t>
-  </si>
-  <si>
-    <t>http://www.eugesta.lt/assets/SOCIALINES-ATSAKOMYBES-ATASKAITA-2016.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/92a17eed-e2f9-e711-8141-e0071b647f61</t>
-  </si>
-  <si>
-    <t>BR50052</t>
-  </si>
-  <si>
-    <t>AB science</t>
-  </si>
-  <si>
-    <t>Healthcare Products</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>27-7-2017</t>
-  </si>
-  <si>
-    <t>Document de Référence 2016</t>
-  </si>
-  <si>
-    <t>http://www.ab-science.com/file_bdd/content/1480493978_DDRVF.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/76787066-df71-e711-812b-e0071b647f61</t>
-  </si>
-  <si>
-    <t>BR50053</t>
-  </si>
-  <si>
-    <t>AB Vassilopoulos</t>
-  </si>
-  <si>
-    <t>Retailers</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>13-1-2020</t>
-  </si>
-  <si>
-    <t>CSR ACTIONS 2016</t>
-  </si>
-  <si>
-    <t>http://globalsustain.org/files/ab-gr-ab_csr-2017_2nd.pdf</t>
-  </si>
-  <si>
-    <t>https://www.ab.gr/responsible/reports</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/57e98d3e-9631-e811-813f-e0071b65f141</t>
-  </si>
-  <si>
-    <t>BR50054</t>
-  </si>
-  <si>
-    <t>ABANCA</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>12-10-2018</t>
-  </si>
-  <si>
-    <t>Memoria Corporativa y de Responsabilidad Social ABANCA 2016</t>
-  </si>
-  <si>
-    <t>In accordance - Comprehensive</t>
-  </si>
-  <si>
-    <t>Content Index Service</t>
-  </si>
-  <si>
-    <t>KPMG</t>
-  </si>
-  <si>
-    <t>https://www.abancacorporacionbancaria.com/files/documents/memoria-anual-rsc-2016-es.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/3bc4a6a3-3345-e711-80ee-3863bb354df0</t>
-  </si>
-  <si>
-    <t>BR50055</t>
-  </si>
-  <si>
-    <t>Abans Electricals PLC</t>
-  </si>
-  <si>
-    <t>Household and Personal Products</t>
-  </si>
-  <si>
-    <t>Sri Lanka</t>
-  </si>
-  <si>
-    <t>DAC-LMICT</t>
-  </si>
-  <si>
-    <t>24-5-2019</t>
-  </si>
-  <si>
-    <t>Annual Report 2016/17</t>
-  </si>
-  <si>
-    <t>https://cdn.cse.lk/cmt/upload_report_file/642_1502793422.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/a413a684-0c7e-e911-a95c-000d3ab6413d</t>
-  </si>
-  <si>
-    <t>BR50056</t>
-  </si>
-  <si>
-    <t>ABB India Ltd.</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>8-2-2018</t>
-  </si>
-  <si>
-    <t>ABB India Annual Report FY 16-17</t>
-  </si>
-  <si>
-    <t>http://www.bseindia.com/bseplus/AnnualReport/500002/5000021216.pdf</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/211d9aa2-1101-e811-8143-e0071b647f61</t>
-  </si>
-  <si>
-    <t>BR50057</t>
-  </si>
-  <si>
-    <t>Abbott</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>Northern America</t>
-  </si>
-  <si>
-    <t>26-7-2017</t>
-  </si>
-  <si>
-    <t>Global Sustainability Report 2016</t>
-  </si>
-  <si>
-    <t>Citing-GRI</t>
-  </si>
-  <si>
-    <t>http://dam.abbott.com/en-us/documents/pdfs/abbott-citizenship/2016_Sustainability_Report_LONG_FORM.pdf</t>
-  </si>
-  <si>
-    <t>http://www.abbott.com/about-abbott/abbott-citizenship/sustainability-reporting.html</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/e6d7ebe6-e267-e711-811e-e0071b65f141</t>
-  </si>
-  <si>
-    <t>BR50058</t>
-  </si>
-  <si>
-    <t>Abbott Ireland</t>
-  </si>
-  <si>
-    <t>Subsidiary</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>13-6-2017</t>
-  </si>
-  <si>
-    <t>2015-2016 Citizenship Report</t>
-  </si>
-  <si>
-    <t>http://dam.abbott.com/en-ie/documents/pdf/2994%20Citizenship%20Report%202016%20v15.pdf</t>
-  </si>
-  <si>
-    <t>http://www.ie.abbott/about-us/global-citizenship/citizenship-reporting.html</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/be1f3ba1-4f50-e711-80f0-3863bb342b20</t>
-  </si>
-  <si>
-    <t>BR50059</t>
-  </si>
-  <si>
-    <t>ABC - AUSTRALIAN BROADCASTING CORPORATION</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Oceania</t>
-  </si>
-  <si>
-    <t>19-10-2018</t>
-  </si>
-  <si>
-    <t>ABC Annual report 2017</t>
-  </si>
-  <si>
-    <t>http://www.abc.net.au/corp/annual-report/2017/documents/ABC_AnnualREport-2017_Volume-1.pdf</t>
-  </si>
-  <si>
-    <t>http://www.abc.net.au/corp/annual-report/2017/home.html</t>
-  </si>
-  <si>
-    <t>http://database.globalreporting.org/reports/e5da35a9-8ed3-e811-8167-e0071b65f141</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AO20"/>
+  <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,1256 +2134,6 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" t="s">
-        <v>140</v>
-      </c>
-      <c r="I11" t="s">
-        <v>133</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" t="s">
-        <v>141</v>
-      </c>
-      <c r="M11" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>74</v>
-      </c>
-      <c r="R11" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" t="s">
-        <v>53</v>
-      </c>
-      <c r="T11" t="s">
-        <v>42</v>
-      </c>
-      <c r="U11" t="s">
-        <v>53</v>
-      </c>
-      <c r="V11" t="s">
-        <v>53</v>
-      </c>
-      <c r="W11" t="s">
-        <v>42</v>
-      </c>
-      <c r="X11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>145</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" t="s">
-        <v>149</v>
-      </c>
-      <c r="J12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" t="s">
-        <v>150</v>
-      </c>
-      <c r="M12" t="s">
-        <v>151</v>
-      </c>
-      <c r="N12" t="s">
-        <v>52</v>
-      </c>
-      <c r="O12" t="s">
-        <v>53</v>
-      </c>
-      <c r="P12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>53</v>
-      </c>
-      <c r="R12" t="s">
-        <v>53</v>
-      </c>
-      <c r="S12" t="s">
-        <v>53</v>
-      </c>
-      <c r="T12" t="s">
-        <v>42</v>
-      </c>
-      <c r="U12" t="s">
-        <v>53</v>
-      </c>
-      <c r="V12" t="s">
-        <v>53</v>
-      </c>
-      <c r="W12" t="s">
-        <v>42</v>
-      </c>
-      <c r="X12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>152</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I13" t="s">
-        <v>157</v>
-      </c>
-      <c r="J13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" t="s">
-        <v>158</v>
-      </c>
-      <c r="M13" t="s">
-        <v>159</v>
-      </c>
-      <c r="N13" t="s">
-        <v>52</v>
-      </c>
-      <c r="O13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P13" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>53</v>
-      </c>
-      <c r="R13" t="s">
-        <v>53</v>
-      </c>
-      <c r="S13" t="s">
-        <v>53</v>
-      </c>
-      <c r="T13" t="s">
-        <v>42</v>
-      </c>
-      <c r="U13" t="s">
-        <v>53</v>
-      </c>
-      <c r="V13" t="s">
-        <v>53</v>
-      </c>
-      <c r="W13" t="s">
-        <v>42</v>
-      </c>
-      <c r="X13" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" t="s">
-        <v>164</v>
-      </c>
-      <c r="I14" t="s">
-        <v>165</v>
-      </c>
-      <c r="J14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" t="s">
-        <v>167</v>
-      </c>
-      <c r="N14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>53</v>
-      </c>
-      <c r="R14" t="s">
-        <v>53</v>
-      </c>
-      <c r="S14" t="s">
-        <v>53</v>
-      </c>
-      <c r="T14" t="s">
-        <v>42</v>
-      </c>
-      <c r="U14" t="s">
-        <v>53</v>
-      </c>
-      <c r="V14" t="s">
-        <v>53</v>
-      </c>
-      <c r="W14" t="s">
-        <v>42</v>
-      </c>
-      <c r="X14" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>168</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>172</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I15" t="s">
-        <v>173</v>
-      </c>
-      <c r="J15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" t="s">
-        <v>174</v>
-      </c>
-      <c r="M15" t="s">
-        <v>175</v>
-      </c>
-      <c r="N15" t="s">
-        <v>52</v>
-      </c>
-      <c r="O15" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>176</v>
-      </c>
-      <c r="R15" t="s">
-        <v>53</v>
-      </c>
-      <c r="S15" t="s">
-        <v>177</v>
-      </c>
-      <c r="T15" t="s">
-        <v>72</v>
-      </c>
-      <c r="U15" t="s">
-        <v>75</v>
-      </c>
-      <c r="V15" t="s">
-        <v>178</v>
-      </c>
-      <c r="W15" t="s">
-        <v>42</v>
-      </c>
-      <c r="X15" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>179</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>182</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I16" t="s">
-        <v>184</v>
-      </c>
-      <c r="J16" t="s">
-        <v>185</v>
-      </c>
-      <c r="K16" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" t="s">
-        <v>186</v>
-      </c>
-      <c r="M16" t="s">
-        <v>187</v>
-      </c>
-      <c r="N16" t="s">
-        <v>52</v>
-      </c>
-      <c r="O16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>53</v>
-      </c>
-      <c r="R16" t="s">
-        <v>53</v>
-      </c>
-      <c r="S16" t="s">
-        <v>53</v>
-      </c>
-      <c r="T16" t="s">
-        <v>42</v>
-      </c>
-      <c r="U16" t="s">
-        <v>53</v>
-      </c>
-      <c r="V16" t="s">
-        <v>53</v>
-      </c>
-      <c r="W16" t="s">
-        <v>42</v>
-      </c>
-      <c r="X16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" t="s">
-        <v>192</v>
-      </c>
-      <c r="I17" t="s">
-        <v>193</v>
-      </c>
-      <c r="J17" t="s">
-        <v>185</v>
-      </c>
-      <c r="K17" t="s">
-        <v>97</v>
-      </c>
-      <c r="L17" t="s">
-        <v>194</v>
-      </c>
-      <c r="M17" t="s">
-        <v>195</v>
-      </c>
-      <c r="N17" t="s">
-        <v>52</v>
-      </c>
-      <c r="O17" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>53</v>
-      </c>
-      <c r="R17" t="s">
-        <v>53</v>
-      </c>
-      <c r="S17" t="s">
-        <v>53</v>
-      </c>
-      <c r="T17" t="s">
-        <v>42</v>
-      </c>
-      <c r="U17" t="s">
-        <v>53</v>
-      </c>
-      <c r="V17" t="s">
-        <v>53</v>
-      </c>
-      <c r="W17" t="s">
-        <v>42</v>
-      </c>
-      <c r="X17" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I18" t="s">
-        <v>200</v>
-      </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" t="s">
-        <v>201</v>
-      </c>
-      <c r="L18" t="s">
-        <v>202</v>
-      </c>
-      <c r="M18" t="s">
-        <v>203</v>
-      </c>
-      <c r="N18" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" t="s">
-        <v>53</v>
-      </c>
-      <c r="P18" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>53</v>
-      </c>
-      <c r="R18" t="s">
-        <v>53</v>
-      </c>
-      <c r="S18" t="s">
-        <v>53</v>
-      </c>
-      <c r="T18" t="s">
-        <v>42</v>
-      </c>
-      <c r="U18" t="s">
-        <v>53</v>
-      </c>
-      <c r="V18" t="s">
-        <v>53</v>
-      </c>
-      <c r="W18" t="s">
-        <v>42</v>
-      </c>
-      <c r="X18" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>205</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>206</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO18" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>208</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>210</v>
-      </c>
-      <c r="G19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" t="s">
-        <v>156</v>
-      </c>
-      <c r="I19" t="s">
-        <v>211</v>
-      </c>
-      <c r="J19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
-        <v>49</v>
-      </c>
-      <c r="L19" t="s">
-        <v>212</v>
-      </c>
-      <c r="M19" t="s">
-        <v>213</v>
-      </c>
-      <c r="N19" t="s">
-        <v>52</v>
-      </c>
-      <c r="O19" t="s">
-        <v>53</v>
-      </c>
-      <c r="P19" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>53</v>
-      </c>
-      <c r="R19" t="s">
-        <v>53</v>
-      </c>
-      <c r="S19" t="s">
-        <v>53</v>
-      </c>
-      <c r="T19" t="s">
-        <v>42</v>
-      </c>
-      <c r="U19" t="s">
-        <v>53</v>
-      </c>
-      <c r="V19" t="s">
-        <v>53</v>
-      </c>
-      <c r="W19" t="s">
-        <v>42</v>
-      </c>
-      <c r="X19" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>214</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>215</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO19" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>217</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>218</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" t="s">
-        <v>219</v>
-      </c>
-      <c r="I20" t="s">
-        <v>220</v>
-      </c>
-      <c r="J20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" t="s">
-        <v>221</v>
-      </c>
-      <c r="L20" t="s">
-        <v>222</v>
-      </c>
-      <c r="M20" t="s">
-        <v>223</v>
-      </c>
-      <c r="N20" t="s">
-        <v>52</v>
-      </c>
-      <c r="O20" t="s">
-        <v>53</v>
-      </c>
-      <c r="P20" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>53</v>
-      </c>
-      <c r="R20" t="s">
-        <v>53</v>
-      </c>
-      <c r="S20" t="s">
-        <v>53</v>
-      </c>
-      <c r="T20" t="s">
-        <v>42</v>
-      </c>
-      <c r="U20" t="s">
-        <v>53</v>
-      </c>
-      <c r="V20" t="s">
-        <v>53</v>
-      </c>
-      <c r="W20" t="s">
-        <v>42</v>
-      </c>
-      <c r="X20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>224</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>225</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO20" t="s">
-        <v>226</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3667,12 +2150,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BD87EC79D7AB454591EAFECBD90626D9" ma:contentTypeVersion="3" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="0d3d7e2407b21afa2d30d9f4658ecfdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a15b57ec-90af-49ba-a0a2-d3f0af0f9931" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a24a46ed92df228c743fe265ed7e3ec" ns2:_="">
     <xsd:import namespace="a15b57ec-90af-49ba-a0a2-d3f0af0f9931"/>
@@ -3810,6 +2287,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F88078F6-43DB-49DB-9553-D1E65F1B4C15}">
   <ds:schemaRefs>
@@ -3819,15 +2302,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D91F3F-1996-4144-8D6F-BAF2247286FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3843,4 +2317,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D55DEAC-2583-419A-AEEA-EE94A1A19F78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>